<commit_message>
modification in create and update api of customers.
</commit_message>
<xml_diff>
--- a/managementcmdfiles/columns.xlsx
+++ b/managementcmdfiles/columns.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5322" uniqueCount="2127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5331" uniqueCount="2127">
   <si>
     <t xml:space="preserve">Column ID</t>
   </si>
@@ -6643,9 +6643,9 @@
   <dimension ref="A1:K1326"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="B76" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="B335" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L76" activeCellId="0" sqref="L76"/>
+      <selection pane="bottomLeft" activeCell="J343" activeCellId="0" sqref="J343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16073,9 +16073,15 @@
       <c r="G343" s="19" t="n">
         <v>480001</v>
       </c>
-      <c r="H343" s="10"/>
-      <c r="I343" s="4"/>
-      <c r="J343" s="7"/>
+      <c r="H343" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I343" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J343" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="K343" s="6"/>
     </row>
     <row r="344" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16100,9 +16106,15 @@
       <c r="G344" s="19" t="n">
         <v>480002</v>
       </c>
-      <c r="H344" s="10"/>
-      <c r="I344" s="4"/>
-      <c r="J344" s="7"/>
+      <c r="H344" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I344" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J344" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="K344" s="6"/>
     </row>
     <row r="345" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16127,9 +16139,15 @@
       <c r="G345" s="19" t="n">
         <v>480003</v>
       </c>
-      <c r="H345" s="10"/>
-      <c r="I345" s="4"/>
-      <c r="J345" s="7"/>
+      <c r="H345" s="10" t="s">
+        <v>670</v>
+      </c>
+      <c r="I345" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J345" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="K345" s="6"/>
     </row>
     <row r="346" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>